<commit_message>
added base classifier wb and added new metaclassifer class
</commit_message>
<xml_diff>
--- a/Results - Combined Classifiers.xlsx
+++ b/Results - Combined Classifiers.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\farha\Documents\GIT\COMP30027-Project-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7C647AE-0012-4165-8C12-7E3934914E7D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9350A0AC-987B-4D1C-ACFF-F0622744A135}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C2E86815-123D-4A73-8760-70182655CD78}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2388" windowHeight="564" activeTab="1" xr2:uid="{C2E86815-123D-4A73-8760-70182655CD78}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="30">
   <si>
     <t>Classifier Combination</t>
   </si>
@@ -97,13 +98,31 @@
   </si>
   <si>
     <t>(MNB, DT, linearSVM)</t>
+  </si>
+  <si>
+    <t>One-R</t>
+  </si>
+  <si>
+    <t>DecisionTree</t>
+  </si>
+  <si>
+    <t>MultinomialNB</t>
+  </si>
+  <si>
+    <t>LinearSVM</t>
+  </si>
+  <si>
+    <t>Classifier(s)</t>
+  </si>
+  <si>
+    <t>Label Spreading</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,8 +154,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Roboto"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -152,6 +176,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCCCCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -237,7 +267,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -270,6 +300,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -586,8 +622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14C1CFAE-63E8-4322-BBA4-D57E44DE5089}">
   <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="H42" sqref="H42"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L41" sqref="L41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1333,4 +1369,251 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5334C64C-F059-41A8-B475-B8CE7B2105CC}">
+  <dimension ref="A1:C21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:C21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="7">
+        <v>0.26930294910000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="7">
+        <v>0.30174262730000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="7">
+        <v>0.31847184989999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="7">
+        <v>0.31745308309999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="7">
+        <v>0.26930294910000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="7">
+        <v>0.31522788200000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="7">
+        <v>0.31061662200000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="7">
+        <v>0.3154959786</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="7">
+        <v>0.26930294910000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="7">
+        <v>0.31056300269999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="7">
+        <v>0.31554959789999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="7">
+        <v>0.32024128689999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="7">
+        <v>0.26930294910000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="7">
+        <v>0.3124128686</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="7">
+        <v>0.3269705094</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="7">
+        <v>0.32254691689999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="13">
+        <v>0.27252010719999997</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="13">
+        <v>0.30726541550000003</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="13">
+        <v>0.31058981229999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="13">
+        <v>0.30474530830000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>